<commit_message>
first draft setup for full day sim
</commit_message>
<xml_diff>
--- a/123NF_topologypaper/init_7.31_busListOrder.xlsx
+++ b/123NF_topologypaper/init_7.31_busListOrder.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaimie\RTlab\runPBCsims\models\sim_123NFunbal\123NF_topologypaper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaimi\Documents\MATLAB\Research\topology_work\experiment_data\models_and_setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77E8A2D-9B01-45D0-A101-D23AD421761A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="600" windowWidth="16920" windowHeight="10200"/>
+    <workbookView xWindow="57510" yWindow="-90" windowWidth="28980" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jaimie.Swartz</author>
   </authors>
   <commentList>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="138">
   <si>
     <t>Test Settings (read this into RTlab)</t>
   </si>
@@ -233,9 +234,6 @@
     <t>83,83,83,57,57,57</t>
   </si>
   <si>
-    <t>2 coloc APNP deep in feeder close together; same siting as suggested by Bolognani (1 coloc halfway down feeder and 1 coloc at node with highest voltage)</t>
-  </si>
-  <si>
     <t>SPBC doesn’t converge</t>
   </si>
   <si>
@@ -272,9 +270,6 @@
     <t>1,2,3,4,5,6,7,8,9,10,11,12,13,14,15</t>
   </si>
   <si>
-    <t>siting Y, nbhd, place apart and more deeply than Bolog siting</t>
-  </si>
-  <si>
     <t>65/P1,65/Q1,65/P2,65/Q2,65/P3,65/Q3</t>
   </si>
   <si>
@@ -425,9 +420,6 @@
     <t>57,56,63,76,87,80</t>
   </si>
   <si>
-    <t>56/P1,57/P1,57/P2,57/P3,63/P1,76/P1,76/P2,76/P3,76/P1,76/P2,76/P3,80/P1,56/Q1,57/Q1,57/Q2,57/Q3,63/Q1,76/Q1,76/Q2,76/Q3,76/Q1,76/Q2,76/Q3,80/Q1</t>
-  </si>
-  <si>
     <t>57_b,57_a,57_b,57_c,57_a,76_a,76_b,76_c,76_a,76_b,76_c,76_b</t>
   </si>
   <si>
@@ -446,9 +438,6 @@
     <t>49_c,49_a,49_a,49_b,49_c,76_a,76_b,76_c,76_a,76_b,76_c,76_b</t>
   </si>
   <si>
-    <t>works too well</t>
-  </si>
-  <si>
     <t>41/P1,45/P1,49/P1,49/P2,49/P3,76/P1,76/P2,76/P3,80/P1,80/P2,80/P3,87/P1,41/Q1,45/Q1,49/Q1,49/Q2,49/Q3,76/Q1,76/Q2,76/Q3,80/Q1,80/Q2,80/Q3,87/Q1</t>
   </si>
   <si>
@@ -474,12 +463,33 @@
   </si>
   <si>
     <t>57/P1,57/P2,57/P3,76/P1,76/P2,76/P3,57/Q1,57/Q2,57/Q3,76/Q1,76/Q2,76/Q3</t>
+  </si>
+  <si>
+    <t>[not in jnl] siting X, coloc, simulate with Helou to verify stable; similar siting as suggested by Bolognani (1 coloc halfway down feeder and 1 coloc at node with highvoltage)</t>
+  </si>
+  <si>
+    <t>[not in jnl] NOT coloc</t>
+  </si>
+  <si>
+    <t>[in jnl] NOT coloc (nbhd), siting Y, placed apart and more deeply than Bolog siting</t>
+  </si>
+  <si>
+    <t>[in jnl] siting X, NOT coloc, simulate with Helou (unstable) and poposed algo (stable); same as test1 except not colocated</t>
+  </si>
+  <si>
+    <t>sitingY_daily</t>
+  </si>
+  <si>
+    <t>11:10-12:20</t>
+  </si>
+  <si>
+    <t>full day sim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -531,7 +541,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -552,12 +562,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -565,6 +569,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,7 +612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -611,12 +627,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -629,116 +639,106 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1024,1147 +1024,1165 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="14" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="17" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" style="17" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.58984375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11.40625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.40625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6796875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="19.26953125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="19.40625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="21.81640625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="16.1328125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" style="12" customWidth="1"/>
+    <col min="13" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:24" s="5" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-    </row>
-    <row r="2" spans="1:13" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+    </row>
+    <row r="2" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="33" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="15" t="s">
+      <c r="F3" s="36"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A4" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="31">
         <v>2</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="31">
         <f>B4+1</f>
         <v>3</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="31">
         <f t="shared" ref="D4:L4" si="0">C4+1</f>
         <v>4</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="31">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="31">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="31">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="31">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="31">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="31">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K4" s="24">
+      <c r="K4" s="31">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="31">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27">
+    <row r="5" spans="1:24" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A5" s="23">
         <v>1</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="18">
         <v>1.25</v>
       </c>
-      <c r="E5" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="K5" s="4">
+      <c r="E5" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="22">
         <v>500</v>
       </c>
-      <c r="L5" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A26" si="1">A5+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>23</v>
+      <c r="C6" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="D6" s="2">
         <v>1.25</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="31" t="s">
+      <c r="E6" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>60</v>
+      <c r="G6" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="K6" s="4">
         <v>500</v>
       </c>
-      <c r="L6" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+      <c r="L6" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A7" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="2">
         <v>1.25</v>
       </c>
-      <c r="E7" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="31" t="s">
+      <c r="E7" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="31" t="s">
+      <c r="G7" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>59</v>
       </c>
       <c r="K7" s="4">
         <v>500</v>
       </c>
-      <c r="L7" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A8" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="2">
         <v>1.25</v>
       </c>
-      <c r="E8" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="31" t="s">
+      <c r="E8" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="J8" s="34" t="s">
-        <v>57</v>
+      <c r="G8" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="K8" s="4">
         <v>500</v>
       </c>
-      <c r="L8" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="44" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29">
+      <c r="L8" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" s="17" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A9" s="18">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="29">
+      <c r="C9" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="18">
         <v>1.25</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="F9" s="41" t="s">
+      <c r="H9" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="I9" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="G9" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="H9" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="I9" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="J9" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="K9" s="43">
+      <c r="J9" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="22">
         <v>500</v>
       </c>
-      <c r="L9" s="40" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="L9" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+    </row>
+    <row r="10" spans="1:24" s="46" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A10" s="40">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B10" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="45">
+      <c r="B10" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="40">
         <v>1.25</v>
       </c>
-      <c r="E10" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" s="48" t="s">
-        <v>116</v>
-      </c>
-      <c r="G10" s="48" t="s">
+      <c r="E10" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="F10" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="48" t="s">
-        <v>117</v>
-      </c>
-      <c r="I10" s="46" t="s">
-        <v>118</v>
-      </c>
-      <c r="J10" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="K10" s="49">
+      <c r="G10" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="I10" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="44">
         <v>500</v>
       </c>
-      <c r="L10" s="50" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L10" s="45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A11" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B11" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>76</v>
+      <c r="B11" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="D11" s="2">
         <v>1.25</v>
       </c>
-      <c r="E11" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="I11" s="34" t="s">
+      <c r="E11" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="15" t="s">
         <v>77</v>
       </c>
+      <c r="G11" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="J11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K11" s="4">
         <v>500</v>
       </c>
-      <c r="L11" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="L11" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A12" s="18">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="18">
         <v>1.25</v>
       </c>
-      <c r="E12" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="K12" s="4">
+      <c r="E12" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="22">
         <v>500</v>
       </c>
-      <c r="L12" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="L12" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A13" s="18">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="18">
         <v>1.25</v>
       </c>
-      <c r="E13" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="G13" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K13" s="4">
+      <c r="E13" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="22">
         <v>500</v>
       </c>
-      <c r="L13" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="L13" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A14" s="18">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="18">
         <v>1.25</v>
       </c>
-      <c r="E14" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="G14" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K14" s="4">
+      <c r="E14" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="K14" s="22">
         <v>500</v>
       </c>
-      <c r="L14" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="L14" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A15" s="18">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="18">
         <v>1.25</v>
       </c>
-      <c r="E15" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="36">
+      <c r="E15" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="28">
         <v>76</v>
       </c>
-      <c r="G15" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" s="36">
+      <c r="G15" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="28">
         <v>76</v>
       </c>
-      <c r="I15" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="J15" s="2" t="s">
+      <c r="I15" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="J15" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="22">
         <v>500</v>
       </c>
-      <c r="L15" s="30" t="s">
-        <v>68</v>
+      <c r="L15" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A16" s="18">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="18">
         <v>1.25</v>
       </c>
-      <c r="E16" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="36" t="s">
+      <c r="E16" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="H16" s="36" t="s">
+      <c r="G16" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K16" s="4">
+      <c r="I16" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16" s="22">
         <v>500</v>
       </c>
-      <c r="L16" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="L16" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A17" s="18">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="18">
         <v>1.25</v>
       </c>
-      <c r="E17" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="36" t="s">
+      <c r="E17" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="H17" s="36" t="s">
+      <c r="G17" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="I17" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K17" s="4">
+      <c r="I17" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17" s="22">
         <v>500</v>
       </c>
-      <c r="L17" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="L17" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A18" s="18">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="18">
         <v>1.25</v>
       </c>
-      <c r="E18" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="36" t="s">
+      <c r="E18" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18" s="36" t="s">
+      <c r="G18" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="I18" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K18" s="4">
+      <c r="I18" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="K18" s="22">
         <v>500</v>
       </c>
-      <c r="L18" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="L18" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A19" s="18">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B19" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="18">
         <v>1.25</v>
       </c>
-      <c r="E19" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="36" t="s">
+      <c r="E19" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="H19" s="36" t="s">
+      <c r="G19" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="H19" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="I19" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K19" s="4">
+      <c r="I19" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="K19" s="22">
         <v>500</v>
       </c>
-      <c r="L19" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="L19" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A20" s="18">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="C20" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="18">
         <v>1.25</v>
       </c>
-      <c r="E20" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="G20" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="H20" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="I20" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="J20" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="K20" s="4">
+      <c r="E20" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" s="22">
         <v>500</v>
       </c>
-      <c r="L20" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="L20" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A21" s="18">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="18">
         <v>1.25</v>
       </c>
-      <c r="E21" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="H21" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="I21" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="J21" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="K21" s="4">
+      <c r="E21" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K21" s="22">
         <v>500</v>
       </c>
-      <c r="L21" s="30" t="s">
-        <v>68</v>
+      <c r="L21" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="59" x14ac:dyDescent="0.75">
       <c r="A22" s="2">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>103</v>
       </c>
       <c r="D22" s="2">
         <v>1.25</v>
       </c>
-      <c r="E22" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="10" t="s">
+      <c r="E22" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G22" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I22" s="13" t="s">
-        <v>115</v>
-      </c>
       <c r="J22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K22" s="4">
         <v>500</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="103.25" x14ac:dyDescent="0.75">
+      <c r="A23" s="18">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B23" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="46" t="s">
-        <v>125</v>
-      </c>
-      <c r="D23" s="45">
+      <c r="B23" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="18">
         <v>1.25</v>
       </c>
-      <c r="E23" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" s="48" t="s">
+      <c r="E23" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G23" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="G23" s="48" t="s">
-        <v>119</v>
-      </c>
-      <c r="H23" s="48" t="s">
+      <c r="H23" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="K23" s="22">
+        <v>500</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M23" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I23" s="46" t="s">
-        <v>127</v>
-      </c>
-      <c r="J23" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="K23" s="49">
-        <v>500</v>
-      </c>
-      <c r="L23" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:13" ht="103.25" x14ac:dyDescent="0.75">
       <c r="A24" s="2">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6">
         <v>1.25</v>
       </c>
-      <c r="E24" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>131</v>
+      <c r="E24" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K24" s="4">
         <v>500</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="59" x14ac:dyDescent="0.75">
       <c r="A25" s="2">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6">
         <v>1</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="13"/>
+        <v>71</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="6"/>
       <c r="J25" s="2"/>
       <c r="K25" s="4">
         <v>500</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="59" x14ac:dyDescent="0.75">
       <c r="A26" s="2">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6">
         <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="13"/>
+        <v>71</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="6"/>
       <c r="J26" s="2"/>
       <c r="K26" s="4">
         <v>500</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="59" x14ac:dyDescent="0.75">
       <c r="A27" s="2">
         <f>A26+1</f>
         <v>23</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8">
+      <c r="C27" s="6"/>
+      <c r="D27" s="6">
         <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="13"/>
+        <v>71</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="59" x14ac:dyDescent="0.75">
       <c r="A28" s="2">
         <f>A27+1</f>
         <v>24</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8">
+      <c r="C28" s="6"/>
+      <c r="D28" s="6">
         <v>1</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="13"/>
+        <v>71</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="59" x14ac:dyDescent="0.75">
       <c r="A29" s="2">
         <f>A28+1</f>
         <v>25</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8">
+      <c r="C29" s="6"/>
+      <c r="D29" s="6">
         <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="13"/>
+        <v>71</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="59" x14ac:dyDescent="0.75">
       <c r="A30" s="2">
         <f>A29+1</f>
         <v>26</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6">
         <v>1</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="16"/>
+        <v>71</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="11"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="L30" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="59" x14ac:dyDescent="0.75">
       <c r="A31" s="2">
         <f>A30+1</f>
         <v>27</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8">
+      <c r="C31" s="6"/>
+      <c r="D31" s="6">
         <v>1</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="16"/>
+        <v>71</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="11"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="L31" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="59" x14ac:dyDescent="0.75">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8">
+      <c r="C32" s="6"/>
+      <c r="D32" s="6">
         <v>1</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="16"/>
+        <v>71</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="11"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="D33" s="8">
+      <c r="L32" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="59" x14ac:dyDescent="0.75">
+      <c r="D33" s="6">
         <v>1</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="L33" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="L33" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="59" x14ac:dyDescent="0.75">
       <c r="E34" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="L34" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="L34" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.75">
       <c r="B41" s="1" t="s">
         <v>45</v>
       </c>
@@ -2181,12 +2199,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>